<commit_message>
Updated Dryness Frequency to be complete for all stations and to produce scatter graphs showing the results
</commit_message>
<xml_diff>
--- a/Outputs/Current Figures/12.6.19_H_C_W_D_index_slopes_avg_r2_pVal_table.xlsx
+++ b/Outputs/Current Figures/12.6.19_H_C_W_D_index_slopes_avg_r2_pVal_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Water\Matt Stone\HIndex_Project\Outputs\Current Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC64C48-B31D-4C28-86C6-994E2AE0975A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE9B654-26E7-44B7-B976-80070857564B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11535" xr2:uid="{23FA91B3-F996-4C7A-951B-0F0CF4FE3AB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13524" xr2:uid="{23FA91B3-F996-4C7A-951B-0F0CF4FE3AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Statitical Analysis" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -181,9 +181,9 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2117,25 +2117,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB2FFBD-811B-40E8-847A-D6CC3FD36130}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
         <v>26</v>
@@ -2162,7 +2162,7 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>0.56499999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>0.92600000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>0.67100000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>0.249</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>0.78800000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>0.69299999999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>0.28799999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3432,6 +3432,72 @@
       </c>
       <c r="Q25">
         <v>0.41699999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <f t="shared" ref="B26:N26" si="0">AVERAGE(B3:B25)</f>
+        <v>-4.4347826086956511E-3</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>86.434782608695656</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>2.1400031817898329E-2</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0.32982608695652171</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>-9.5217391304347806E-3</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>20.065217391304355</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>2.9932700917776386E-2</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>0.26573913043478259</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>4.6956521739130435E-3</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>14.243478260869566</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>1.3986133878871407E-2</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>0.40052173913043476</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>1.2173913043478262E-3</v>
+      </c>
+      <c r="O26">
+        <f>AVERAGE(O3:O25)</f>
+        <v>9.5695652173913057</v>
+      </c>
+      <c r="P26">
+        <f t="shared" ref="P26:Q26" si="1">AVERAGE(P3:P25)</f>
+        <v>9.2968816474342658E-3</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="1"/>
+        <v>0.57578260869565212</v>
       </c>
     </row>
   </sheetData>
@@ -3459,9 +3525,9 @@
       <selection activeCell="I130" sqref="I130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -3535,7 +3601,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1890</v>
       </c>
@@ -3609,7 +3675,7 @@
         <v>85.28</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1891</v>
       </c>
@@ -3683,7 +3749,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1892</v>
       </c>
@@ -3757,7 +3823,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1893</v>
       </c>
@@ -3831,7 +3897,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1894</v>
       </c>
@@ -3905,7 +3971,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1895</v>
       </c>
@@ -3979,7 +4045,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1896</v>
       </c>
@@ -4053,7 +4119,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1897</v>
       </c>
@@ -4127,7 +4193,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1898</v>
       </c>
@@ -4201,7 +4267,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1899</v>
       </c>
@@ -4275,7 +4341,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1900</v>
       </c>
@@ -4349,7 +4415,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1901</v>
       </c>
@@ -4423,7 +4489,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1902</v>
       </c>
@@ -4497,7 +4563,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1903</v>
       </c>
@@ -4571,7 +4637,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1904</v>
       </c>
@@ -4645,7 +4711,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1905</v>
       </c>
@@ -4719,7 +4785,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1906</v>
       </c>
@@ -4793,7 +4859,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1907</v>
       </c>
@@ -4867,7 +4933,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1908</v>
       </c>
@@ -4941,7 +5007,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1909</v>
       </c>
@@ -5015,7 +5081,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1910</v>
       </c>
@@ -5089,7 +5155,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1911</v>
       </c>
@@ -5163,7 +5229,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1912</v>
       </c>
@@ -5237,7 +5303,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1913</v>
       </c>
@@ -5311,7 +5377,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1914</v>
       </c>
@@ -5385,7 +5451,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1915</v>
       </c>
@@ -5459,7 +5525,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1916</v>
       </c>
@@ -5533,7 +5599,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1917</v>
       </c>
@@ -5607,7 +5673,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1918</v>
       </c>
@@ -5681,7 +5747,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1919</v>
       </c>
@@ -5755,7 +5821,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1920</v>
       </c>
@@ -5829,7 +5895,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1921</v>
       </c>
@@ -5903,7 +5969,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1922</v>
       </c>
@@ -5977,7 +6043,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1923</v>
       </c>
@@ -6051,7 +6117,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1924</v>
       </c>
@@ -6125,7 +6191,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1925</v>
       </c>
@@ -6199,7 +6265,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1926</v>
       </c>
@@ -6273,7 +6339,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1927</v>
       </c>
@@ -6347,7 +6413,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1928</v>
       </c>
@@ -6421,7 +6487,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1929</v>
       </c>
@@ -6495,7 +6561,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1930</v>
       </c>
@@ -6569,7 +6635,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1931</v>
       </c>
@@ -6643,7 +6709,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1932</v>
       </c>
@@ -6717,7 +6783,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1933</v>
       </c>
@@ -6791,7 +6857,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1934</v>
       </c>
@@ -6865,7 +6931,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1935</v>
       </c>
@@ -6939,7 +7005,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1936</v>
       </c>
@@ -7013,7 +7079,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1937</v>
       </c>
@@ -7087,7 +7153,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1938</v>
       </c>
@@ -7161,7 +7227,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1939</v>
       </c>
@@ -7235,7 +7301,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1940</v>
       </c>
@@ -7309,7 +7375,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1941</v>
       </c>
@@ -7383,7 +7449,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1942</v>
       </c>
@@ -7457,7 +7523,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1943</v>
       </c>
@@ -7531,7 +7597,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1944</v>
       </c>
@@ -7605,7 +7671,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1945</v>
       </c>
@@ -7679,7 +7745,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1946</v>
       </c>
@@ -7753,7 +7819,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1947</v>
       </c>
@@ -7827,7 +7893,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1948</v>
       </c>
@@ -7901,7 +7967,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1949</v>
       </c>
@@ -7975,7 +8041,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1950</v>
       </c>
@@ -8049,7 +8115,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1951</v>
       </c>
@@ -8123,7 +8189,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>1952</v>
       </c>
@@ -8197,7 +8263,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1953</v>
       </c>
@@ -8271,7 +8337,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1954</v>
       </c>
@@ -8345,7 +8411,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1955</v>
       </c>
@@ -8419,7 +8485,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1956</v>
       </c>
@@ -8493,7 +8559,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>1957</v>
       </c>
@@ -8567,7 +8633,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1958</v>
       </c>
@@ -8641,7 +8707,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1959</v>
       </c>
@@ -8715,7 +8781,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>1960</v>
       </c>
@@ -8789,7 +8855,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1961</v>
       </c>
@@ -8863,7 +8929,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1962</v>
       </c>
@@ -8937,7 +9003,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1963</v>
       </c>
@@ -9011,7 +9077,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1964</v>
       </c>
@@ -9085,7 +9151,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>1965</v>
       </c>
@@ -9159,7 +9225,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1966</v>
       </c>
@@ -9233,7 +9299,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1967</v>
       </c>
@@ -9307,7 +9373,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1968</v>
       </c>
@@ -9381,7 +9447,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1969</v>
       </c>
@@ -9455,7 +9521,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1970</v>
       </c>
@@ -9529,7 +9595,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>1971</v>
       </c>
@@ -9603,7 +9669,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1972</v>
       </c>
@@ -9677,7 +9743,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1973</v>
       </c>
@@ -9751,7 +9817,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>1974</v>
       </c>
@@ -9825,7 +9891,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>1975</v>
       </c>
@@ -9899,7 +9965,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1976</v>
       </c>
@@ -9973,7 +10039,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>1977</v>
       </c>
@@ -10047,7 +10113,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1978</v>
       </c>
@@ -10121,7 +10187,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>1979</v>
       </c>
@@ -10195,7 +10261,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>1980</v>
       </c>
@@ -10269,7 +10335,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>1981</v>
       </c>
@@ -10343,7 +10409,7 @@
         <v>84.91</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>1982</v>
       </c>
@@ -10417,7 +10483,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>1983</v>
       </c>
@@ -10491,7 +10557,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1984</v>
       </c>
@@ -10565,7 +10631,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1985</v>
       </c>
@@ -10639,7 +10705,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>1986</v>
       </c>
@@ -10713,7 +10779,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1987</v>
       </c>
@@ -10787,7 +10853,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>1988</v>
       </c>
@@ -10861,7 +10927,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1989</v>
       </c>
@@ -10935,7 +11001,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>1990</v>
       </c>
@@ -11009,7 +11075,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1991</v>
       </c>
@@ -11083,7 +11149,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1992</v>
       </c>
@@ -11157,7 +11223,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1993</v>
       </c>
@@ -11231,7 +11297,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1994</v>
       </c>
@@ -11305,7 +11371,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1995</v>
       </c>
@@ -11379,7 +11445,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1996</v>
       </c>
@@ -11453,7 +11519,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1997</v>
       </c>
@@ -11527,7 +11593,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1998</v>
       </c>
@@ -11601,7 +11667,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>1999</v>
       </c>
@@ -11675,7 +11741,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2000</v>
       </c>
@@ -11749,7 +11815,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2001</v>
       </c>
@@ -11823,7 +11889,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2002</v>
       </c>
@@ -11897,7 +11963,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2003</v>
       </c>
@@ -11971,7 +12037,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2004</v>
       </c>
@@ -12045,7 +12111,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2005</v>
       </c>
@@ -12119,7 +12185,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2006</v>
       </c>
@@ -12193,7 +12259,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2007</v>
       </c>
@@ -12267,7 +12333,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2008</v>
       </c>
@@ -12341,7 +12407,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2009</v>
       </c>
@@ -12415,7 +12481,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2010</v>
       </c>
@@ -12489,7 +12555,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2011</v>
       </c>
@@ -12563,7 +12629,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2012</v>
       </c>
@@ -12637,7 +12703,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2013</v>
       </c>

</xml_diff>

<commit_message>
created plots for 1981-2010/2013 for W, C, and H index. Compared these results to POR plots. Did linear statistical analysis of 1981-2010/2013 period.
</commit_message>
<xml_diff>
--- a/Outputs/Current Figures/12.6.19_H_C_W_D_index_slopes_avg_r2_pVal_table.xlsx
+++ b/Outputs/Current Figures/12.6.19_H_C_W_D_index_slopes_avg_r2_pVal_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Water\Matt Stone\HIndex_Project\Outputs\Current Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE9B654-26E7-44B7-B976-80070857564B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB10721-9766-4EB1-BD76-6FD88D7A6F75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13524" xr2:uid="{23FA91B3-F996-4C7A-951B-0F0CF4FE3AB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11535" xr2:uid="{23FA91B3-F996-4C7A-951B-0F0CF4FE3AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Statitical Analysis" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,197 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2120,22 +2310,22 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y9" sqref="Y9"/>
+      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="5" t="s">
         <v>26</v>
@@ -2162,7 +2352,7 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2215,7 +2405,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2268,7 +2458,7 @@
         <v>0.56499999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2321,7 +2511,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2374,7 +2564,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2427,7 +2617,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2480,7 +2670,7 @@
         <v>0.92600000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2533,7 +2723,7 @@
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2586,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2639,7 +2829,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2692,7 +2882,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2745,7 +2935,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2798,7 +2988,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2851,7 +3041,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2904,7 +3094,7 @@
         <v>0.67100000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2957,7 +3147,7 @@
         <v>0.249</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3010,7 +3200,7 @@
         <v>0.78800000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -3063,7 +3253,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -3116,7 +3306,7 @@
         <v>0.69299999999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -3169,7 +3359,7 @@
         <v>0.71699999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -3222,7 +3412,7 @@
         <v>0.28799999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -3275,7 +3465,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3328,7 +3518,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -3381,7 +3571,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3434,7 +3624,7 @@
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" ref="B26:N26" si="0">AVERAGE(B3:B25)</f>
         <v>-4.4347826086956511E-3</v>
@@ -3508,8 +3698,24 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D25 H3:H25 L3:L25 P3:P25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
       <formula>"0..5"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E26 I3:I26 M3:M26 Q3:Q26">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="between">
+      <formula>0.05</formula>
+      <formula>0.06</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="between">
+      <formula>0.04</formula>
+      <formula>0.04</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3525,9 +3731,9 @@
       <selection activeCell="I130" sqref="I130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -3601,7 +3807,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1890</v>
       </c>
@@ -3675,7 +3881,7 @@
         <v>85.28</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1891</v>
       </c>
@@ -3749,7 +3955,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1892</v>
       </c>
@@ -3823,7 +4029,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1893</v>
       </c>
@@ -3897,7 +4103,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1894</v>
       </c>
@@ -3971,7 +4177,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1895</v>
       </c>
@@ -4045,7 +4251,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1896</v>
       </c>
@@ -4119,7 +4325,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1897</v>
       </c>
@@ -4193,7 +4399,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1898</v>
       </c>
@@ -4267,7 +4473,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1899</v>
       </c>
@@ -4341,7 +4547,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1900</v>
       </c>
@@ -4415,7 +4621,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1901</v>
       </c>
@@ -4489,7 +4695,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1902</v>
       </c>
@@ -4563,7 +4769,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1903</v>
       </c>
@@ -4637,7 +4843,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1904</v>
       </c>
@@ -4711,7 +4917,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1905</v>
       </c>
@@ -4785,7 +4991,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1906</v>
       </c>
@@ -4859,7 +5065,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1907</v>
       </c>
@@ -4933,7 +5139,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1908</v>
       </c>
@@ -5007,7 +5213,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1909</v>
       </c>
@@ -5081,7 +5287,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1910</v>
       </c>
@@ -5155,7 +5361,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1911</v>
       </c>
@@ -5229,7 +5435,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1912</v>
       </c>
@@ -5303,7 +5509,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1913</v>
       </c>
@@ -5377,7 +5583,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1914</v>
       </c>
@@ -5451,7 +5657,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1915</v>
       </c>
@@ -5525,7 +5731,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1916</v>
       </c>
@@ -5599,7 +5805,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1917</v>
       </c>
@@ -5673,7 +5879,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1918</v>
       </c>
@@ -5747,7 +5953,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1919</v>
       </c>
@@ -5821,7 +6027,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1920</v>
       </c>
@@ -5895,7 +6101,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1921</v>
       </c>
@@ -5969,7 +6175,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1922</v>
       </c>
@@ -6043,7 +6249,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1923</v>
       </c>
@@ -6117,7 +6323,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1924</v>
       </c>
@@ -6191,7 +6397,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1925</v>
       </c>
@@ -6265,7 +6471,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1926</v>
       </c>
@@ -6339,7 +6545,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1927</v>
       </c>
@@ -6413,7 +6619,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1928</v>
       </c>
@@ -6487,7 +6693,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1929</v>
       </c>
@@ -6561,7 +6767,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1930</v>
       </c>
@@ -6635,7 +6841,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1931</v>
       </c>
@@ -6709,7 +6915,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1932</v>
       </c>
@@ -6783,7 +6989,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1933</v>
       </c>
@@ -6857,7 +7063,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1934</v>
       </c>
@@ -6931,7 +7137,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1935</v>
       </c>
@@ -7005,7 +7211,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1936</v>
       </c>
@@ -7079,7 +7285,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1937</v>
       </c>
@@ -7153,7 +7359,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1938</v>
       </c>
@@ -7227,7 +7433,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1939</v>
       </c>
@@ -7301,7 +7507,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1940</v>
       </c>
@@ -7375,7 +7581,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1941</v>
       </c>
@@ -7449,7 +7655,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1942</v>
       </c>
@@ -7523,7 +7729,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1943</v>
       </c>
@@ -7597,7 +7803,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1944</v>
       </c>
@@ -7671,7 +7877,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1945</v>
       </c>
@@ -7745,7 +7951,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1946</v>
       </c>
@@ -7819,7 +8025,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1947</v>
       </c>
@@ -7893,7 +8099,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1948</v>
       </c>
@@ -7967,7 +8173,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1949</v>
       </c>
@@ -8041,7 +8247,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1950</v>
       </c>
@@ -8115,7 +8321,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1951</v>
       </c>
@@ -8189,7 +8395,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1952</v>
       </c>
@@ -8263,7 +8469,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1953</v>
       </c>
@@ -8337,7 +8543,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1954</v>
       </c>
@@ -8411,7 +8617,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1955</v>
       </c>
@@ -8485,7 +8691,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1956</v>
       </c>
@@ -8559,7 +8765,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1957</v>
       </c>
@@ -8633,7 +8839,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1958</v>
       </c>
@@ -8707,7 +8913,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1959</v>
       </c>
@@ -8781,7 +8987,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1960</v>
       </c>
@@ -8855,7 +9061,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1961</v>
       </c>
@@ -8929,7 +9135,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1962</v>
       </c>
@@ -9003,7 +9209,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1963</v>
       </c>
@@ -9077,7 +9283,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1964</v>
       </c>
@@ -9151,7 +9357,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1965</v>
       </c>
@@ -9225,7 +9431,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1966</v>
       </c>
@@ -9299,7 +9505,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1967</v>
       </c>
@@ -9373,7 +9579,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1968</v>
       </c>
@@ -9447,7 +9653,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1969</v>
       </c>
@@ -9521,7 +9727,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1970</v>
       </c>
@@ -9595,7 +9801,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1971</v>
       </c>
@@ -9669,7 +9875,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1972</v>
       </c>
@@ -9743,7 +9949,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1973</v>
       </c>
@@ -9817,7 +10023,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1974</v>
       </c>
@@ -9891,7 +10097,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1975</v>
       </c>
@@ -9965,7 +10171,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1976</v>
       </c>
@@ -10039,7 +10245,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1977</v>
       </c>
@@ -10113,7 +10319,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1978</v>
       </c>
@@ -10187,7 +10393,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1979</v>
       </c>
@@ -10261,7 +10467,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1980</v>
       </c>
@@ -10335,7 +10541,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1981</v>
       </c>
@@ -10409,7 +10615,7 @@
         <v>84.91</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1982</v>
       </c>
@@ -10483,7 +10689,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1983</v>
       </c>
@@ -10557,7 +10763,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1984</v>
       </c>
@@ -10631,7 +10837,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1985</v>
       </c>
@@ -10705,7 +10911,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1986</v>
       </c>
@@ -10779,7 +10985,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1987</v>
       </c>
@@ -10853,7 +11059,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1988</v>
       </c>
@@ -10927,7 +11133,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1989</v>
       </c>
@@ -11001,7 +11207,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1990</v>
       </c>
@@ -11075,7 +11281,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1991</v>
       </c>
@@ -11149,7 +11355,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1992</v>
       </c>
@@ -11223,7 +11429,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1993</v>
       </c>
@@ -11297,7 +11503,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1994</v>
       </c>
@@ -11371,7 +11577,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1995</v>
       </c>
@@ -11445,7 +11651,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1996</v>
       </c>
@@ -11519,7 +11725,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1997</v>
       </c>
@@ -11593,7 +11799,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1998</v>
       </c>
@@ -11667,7 +11873,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1999</v>
       </c>
@@ -11741,7 +11947,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2000</v>
       </c>
@@ -11815,7 +12021,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2001</v>
       </c>
@@ -11889,7 +12095,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2002</v>
       </c>
@@ -11963,7 +12169,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2003</v>
       </c>
@@ -12037,7 +12243,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2004</v>
       </c>
@@ -12111,7 +12317,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2005</v>
       </c>
@@ -12185,7 +12391,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2006</v>
       </c>
@@ -12259,7 +12465,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2007</v>
       </c>
@@ -12333,7 +12539,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2008</v>
       </c>
@@ -12407,7 +12613,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2009</v>
       </c>
@@ -12481,7 +12687,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2010</v>
       </c>
@@ -12555,7 +12761,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2011</v>
       </c>
@@ -12629,7 +12835,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2012</v>
       </c>
@@ -12703,7 +12909,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2013</v>
       </c>

</xml_diff>

<commit_message>
Updated HIndex Main to have a more flexible year setting and added a function to calculate the spearman and Kendall coefficients
</commit_message>
<xml_diff>
--- a/Outputs/Current Figures/12.6.19_H_C_W_D_index_slopes_avg_r2_pVal_table.xlsx
+++ b/Outputs/Current Figures/12.6.19_H_C_W_D_index_slopes_avg_r2_pVal_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Water\Matt Stone\HIndex_Project\Outputs\Current Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB10721-9766-4EB1-BD76-6FD88D7A6F75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82945C1-7C3C-45BD-AF76-729137B990B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11535" xr2:uid="{23FA91B3-F996-4C7A-951B-0F0CF4FE3AB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13524" xr2:uid="{23FA91B3-F996-4C7A-951B-0F0CF4FE3AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Statitical Analysis" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
   <si>
     <t>a_Saint Francis_19082012</t>
   </si>
@@ -115,24 +115,37 @@
     <t>W-Index</t>
   </si>
   <si>
-    <t>D-Index</t>
+    <t>Year</t>
   </si>
   <si>
-    <t>R Squared</t>
+    <t>r pValue</t>
   </si>
   <si>
-    <t>pValue</t>
+    <t>r</t>
   </si>
   <si>
-    <t>Year</t>
+    <t>r^2</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>rho pValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tau </t>
+  </si>
+  <si>
+    <t>tau pValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -178,20 +191,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -219,156 +233,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2307,52 +2171,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB2FFBD-811B-40E8-847A-D6CC3FD36130}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
+      <selection pane="bottomRight" activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+    </row>
+    <row r="2" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2363,1359 +2243,2086 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" s="1"/>
+    </row>
+    <row r="3" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>-8.0000000000000002E-3</v>
       </c>
-      <c r="C3" s="1">
-        <v>86</v>
+      <c r="C3" s="5">
+        <v>85.9</v>
       </c>
       <c r="D3" s="2">
+        <v>-0.119721266498277</v>
+      </c>
+      <c r="E3">
         <v>1.4333181651954701E-2</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3">
         <v>0.224</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3">
+        <v>-0.12833338763513399</v>
+      </c>
+      <c r="H3">
+        <v>0.19199960596931301</v>
+      </c>
+      <c r="I3">
+        <v>-9.3812793004779196E-2</v>
+      </c>
+      <c r="J3">
+        <v>0.18195199470557799</v>
+      </c>
+      <c r="K3">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="G3" s="1">
+      <c r="L3" s="6">
         <v>22.6</v>
       </c>
-      <c r="H3" s="3">
+      <c r="M3">
         <v>5.0898768097019098E-2</v>
       </c>
-      <c r="I3" s="1">
+      <c r="N3">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="J3">
+      <c r="O3">
+        <v>-0.217338672091896</v>
+      </c>
+      <c r="P3">
+        <v>2.5941081054135701E-2</v>
+      </c>
+      <c r="Q3">
+        <v>-0.14881637744047899</v>
+      </c>
+      <c r="R3">
+        <v>3.0818499431161401E-2</v>
+      </c>
+      <c r="S3">
+        <v>-0.22560755328006599</v>
+      </c>
+      <c r="T3">
         <v>-0.01</v>
       </c>
-      <c r="K3">
+      <c r="U3" s="6">
         <v>11.2</v>
       </c>
-      <c r="L3" s="4">
+      <c r="V3">
+        <v>-0.17252852686730599</v>
+      </c>
+      <c r="W3">
         <v>2.9766092583003001E-2</v>
       </c>
-      <c r="M3">
+      <c r="X3">
         <v>7.8E-2</v>
       </c>
-      <c r="N3">
-        <v>2E-3</v>
-      </c>
-      <c r="O3">
-        <v>9.9</v>
-      </c>
-      <c r="P3" s="4">
-        <v>3.2332523125884198E-3</v>
-      </c>
-      <c r="Q3">
-        <v>0.56499999999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y3">
+        <v>-0.160907743194871</v>
+      </c>
+      <c r="Z3">
+        <v>0.10105083278392001</v>
+      </c>
+      <c r="AA3">
+        <v>-0.10223525787148</v>
+      </c>
+      <c r="AB3">
+        <v>0.12300183087399399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>-1.2999999999999999E-2</v>
       </c>
-      <c r="C4" s="1">
-        <v>85</v>
+      <c r="C4" s="5">
+        <v>85.1</v>
       </c>
       <c r="D4" s="2">
+        <v>-0.20250572274886</v>
+      </c>
+      <c r="E4">
         <v>4.1008567746052202E-2</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4">
         <v>3.1E-2</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4">
+        <v>-0.213217065499436</v>
+      </c>
+      <c r="H4">
+        <v>2.2744180901620802E-2</v>
+      </c>
+      <c r="I4">
+        <v>-0.13877237890948199</v>
+      </c>
+      <c r="J4">
+        <v>3.8786536113427798E-2</v>
+      </c>
+      <c r="K4">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G4" s="1">
+      <c r="L4" s="6">
         <v>23.1</v>
       </c>
-      <c r="H4" s="3">
+      <c r="M4">
         <v>6.9817965362211102E-3</v>
       </c>
-      <c r="I4" s="1">
+      <c r="N4">
         <v>0.377</v>
       </c>
-      <c r="J4">
+      <c r="O4">
+        <v>4.0736654558097399E-2</v>
+      </c>
+      <c r="P4">
+        <v>0.66695287703956396</v>
+      </c>
+      <c r="Q4">
+        <v>3.12091440773699E-2</v>
+      </c>
+      <c r="R4">
+        <v>0.63937393920478702</v>
+      </c>
+      <c r="S4">
+        <v>8.3557145333125499E-2</v>
+      </c>
+      <c r="T4">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="K4">
+      <c r="U4" s="6">
         <v>11.6</v>
       </c>
-      <c r="L4" s="4">
+      <c r="V4">
+        <v>0.118133792439682</v>
+      </c>
+      <c r="W4">
         <v>1.39555929161816E-2</v>
       </c>
-      <c r="M4">
+      <c r="X4">
         <v>0.21099999999999999</v>
       </c>
-      <c r="N4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="O4">
-        <v>9.9</v>
-      </c>
-      <c r="P4" s="4">
-        <v>2.62197837254445E-2</v>
-      </c>
-      <c r="Q4">
-        <v>8.5000000000000006E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y4">
+        <v>0.107901329083366</v>
+      </c>
+      <c r="Z4">
+        <v>0.25315726960150597</v>
+      </c>
+      <c r="AA4">
+        <v>7.2388360213493902E-2</v>
+      </c>
+      <c r="AB4">
+        <v>0.25480708797449803</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
         <v>-1E-3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <v>86</v>
       </c>
       <c r="D5" s="2">
+        <v>-1.51916891215833E-2</v>
+      </c>
+      <c r="E5">
         <v>2.3078741836701799E-4</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5">
         <v>0.86899999999999999</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5">
+        <v>-1.1776222714112701E-2</v>
+      </c>
+      <c r="H5">
+        <v>0.89799206387124797</v>
+      </c>
+      <c r="I5">
+        <v>-1.35509047737841E-2</v>
+      </c>
+      <c r="J5">
+        <v>0.83390293432454299</v>
+      </c>
+      <c r="K5">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="G5" s="1">
+      <c r="L5" s="6">
         <v>23.3</v>
       </c>
-      <c r="H5" s="3">
+      <c r="M5">
         <v>1.4866915868738701E-3</v>
       </c>
-      <c r="I5" s="1">
+      <c r="N5">
         <v>0.67500000000000004</v>
       </c>
-      <c r="J5">
+      <c r="O5">
+        <v>-3.4366182801769798E-2</v>
+      </c>
+      <c r="P5">
+        <v>0.70824462478327399</v>
+      </c>
+      <c r="Q5">
+        <v>-2.1969604333679001E-2</v>
+      </c>
+      <c r="R5">
+        <v>0.73062800635916103</v>
+      </c>
+      <c r="S5">
+        <v>-3.8557639799059497E-2</v>
+      </c>
+      <c r="T5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K5">
+      <c r="U5" s="6">
         <v>12.2</v>
       </c>
-      <c r="L5" s="4">
+      <c r="V5">
+        <v>5.1519600870985498E-2</v>
+      </c>
+      <c r="W5">
         <v>2.6542692739057699E-3</v>
       </c>
-      <c r="M5">
+      <c r="X5">
         <v>0.57499999999999996</v>
       </c>
-      <c r="N5">
-        <v>1E-3</v>
-      </c>
-      <c r="O5">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="P5" s="4">
-        <v>5.9724698754304295E-4</v>
-      </c>
-      <c r="Q5">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y5">
+        <v>8.8742264693627906E-2</v>
+      </c>
+      <c r="Z5">
+        <v>0.333072511634394</v>
+      </c>
+      <c r="AA5">
+        <v>6.2284695965575003E-2</v>
+      </c>
+      <c r="AB5">
+        <v>0.31231013771744498</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="C6" s="1">
-        <v>86</v>
+      <c r="C6" s="5">
+        <v>86.2</v>
       </c>
       <c r="D6" s="2">
+        <v>-6.7018738434123398E-2</v>
+      </c>
+      <c r="E6">
         <v>4.4915113013045396E-3</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6">
         <v>0.46100000000000002</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6">
+        <v>-6.2130651470703499E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.49480489330180799</v>
+      </c>
+      <c r="I6">
+        <v>-4.8251169795285598E-2</v>
+      </c>
+      <c r="J6">
+        <v>0.450784693641406</v>
+      </c>
+      <c r="K6">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="G6" s="1">
+      <c r="L6" s="6">
         <v>22.6</v>
       </c>
-      <c r="H6" s="3">
+      <c r="M6">
         <v>7.1848099821173496E-3</v>
       </c>
-      <c r="I6" s="1">
+      <c r="N6">
         <v>0.35099999999999998</v>
       </c>
-      <c r="J6">
+      <c r="O6">
+        <v>-0.114539244478619</v>
+      </c>
+      <c r="P6">
+        <v>0.207133262612197</v>
+      </c>
+      <c r="Q6">
+        <v>-7.0984016439417805E-2</v>
+      </c>
+      <c r="R6">
+        <v>0.26167078219583401</v>
+      </c>
+      <c r="S6">
+        <v>-8.4763258444428599E-2</v>
+      </c>
+      <c r="T6">
         <v>2E-3</v>
       </c>
-      <c r="K6">
+      <c r="U6" s="6">
         <v>13.1</v>
       </c>
-      <c r="L6" s="4">
+      <c r="V6">
+        <v>2.98899414628979E-2</v>
+      </c>
+      <c r="W6">
         <v>8.9340860065545403E-4</v>
       </c>
-      <c r="M6">
+      <c r="X6">
         <v>0.74299999999999999</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>9.6</v>
-      </c>
-      <c r="P6" s="4">
-        <v>2.1233218330252201E-5</v>
-      </c>
-      <c r="Q6">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y6">
+        <v>-8.8030865634566805E-3</v>
+      </c>
+      <c r="Z6">
+        <v>0.92301549469266198</v>
+      </c>
+      <c r="AA6">
+        <v>-1.0668802347905E-2</v>
+      </c>
+      <c r="AB6">
+        <v>0.86288336826405299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>1.2E-2</v>
       </c>
-      <c r="C7" s="1">
-        <v>84</v>
+      <c r="C7" s="5">
+        <v>84.2</v>
       </c>
       <c r="D7" s="2">
+        <v>0.22975090289557101</v>
+      </c>
+      <c r="E7">
         <v>5.2785477381347201E-2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7">
         <v>0.01</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7">
+        <v>0.22552345707558599</v>
+      </c>
+      <c r="H7">
+        <v>1.17882081430479E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.160472321950095</v>
+      </c>
+      <c r="J7">
+        <v>1.2966413187193699E-2</v>
+      </c>
+      <c r="K7">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="G7" s="1">
+      <c r="L7" s="6">
         <v>21.8</v>
       </c>
-      <c r="H7" s="3">
+      <c r="M7">
         <v>5.0817378432232996E-3</v>
       </c>
-      <c r="I7" s="1">
+      <c r="N7">
         <v>0.43099999999999999</v>
       </c>
-      <c r="J7">
+      <c r="O7">
+        <v>-8.2290475831606397E-2</v>
+      </c>
+      <c r="P7">
+        <v>0.36355618273296297</v>
+      </c>
+      <c r="Q7">
+        <v>-5.6546768577781799E-2</v>
+      </c>
+      <c r="R7">
+        <v>0.37094790141796502</v>
+      </c>
+      <c r="S7">
+        <v>-7.1286308946551302E-2</v>
+      </c>
+      <c r="T7">
         <v>0.01</v>
       </c>
-      <c r="K7">
+      <c r="U7" s="6">
         <v>16</v>
       </c>
-      <c r="L7" s="4">
+      <c r="V7">
+        <v>0.15515690524540901</v>
+      </c>
+      <c r="W7">
         <v>2.40736652453327E-2</v>
       </c>
-      <c r="M7">
+      <c r="X7">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="P7" s="4">
-        <v>7.1846567852640306E-5</v>
-      </c>
-      <c r="Q7">
-        <v>0.92600000000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y7">
+        <v>0.16261365174904199</v>
+      </c>
+      <c r="Z7">
+        <v>7.1156038849105499E-2</v>
+      </c>
+      <c r="AA7">
+        <v>0.114128304784479</v>
+      </c>
+      <c r="AB7">
+        <v>6.0533392493645498E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="C8" s="1">
-        <v>84</v>
+      <c r="C8" s="5">
+        <v>84.1</v>
       </c>
       <c r="D8" s="2">
+        <v>-0.294402536700693</v>
+      </c>
+      <c r="E8">
         <v>8.6672853615814102E-2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8">
         <v>1E-3</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8">
+        <v>-0.31792846716740297</v>
+      </c>
+      <c r="H8">
+        <v>4.50967899594142E-4</v>
+      </c>
+      <c r="I8">
+        <v>-0.223976606118623</v>
+      </c>
+      <c r="J8">
+        <v>7.0280750104365899E-4</v>
+      </c>
+      <c r="K8">
         <v>-1.6E-2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="L8" s="6">
         <v>20.6</v>
       </c>
-      <c r="H8" s="3">
+      <c r="M8">
         <v>2.78438416181441E-2</v>
       </c>
-      <c r="I8" s="1">
+      <c r="N8">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="J8">
+      <c r="O8">
+        <v>-0.15130211461093801</v>
+      </c>
+      <c r="P8">
+        <v>0.101945195974102</v>
+      </c>
+      <c r="Q8">
+        <v>-0.10449369936731399</v>
+      </c>
+      <c r="R8">
+        <v>0.105290123734464</v>
+      </c>
+      <c r="S8">
+        <v>-0.166864740488049</v>
+      </c>
+      <c r="T8">
         <v>2E-3</v>
       </c>
-      <c r="K8">
+      <c r="U8" s="6">
         <v>16.3</v>
       </c>
-      <c r="L8" s="4">
+      <c r="V8">
+        <v>3.88548365992437E-2</v>
+      </c>
+      <c r="W8">
         <v>1.5096983271538601E-3</v>
       </c>
-      <c r="M8">
+      <c r="X8">
         <v>0.67600000000000005</v>
       </c>
-      <c r="N8">
-        <v>1E-3</v>
-      </c>
-      <c r="O8">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="P8" s="4">
-        <v>3.1642069385496899E-3</v>
-      </c>
-      <c r="Q8">
-        <v>0.54500000000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y8">
+        <v>5.2937008797404102E-2</v>
+      </c>
+      <c r="Z8">
+        <v>0.56913826860390404</v>
+      </c>
+      <c r="AA8">
+        <v>4.0724641530369601E-2</v>
+      </c>
+      <c r="AB8">
+        <v>0.51487433666664895</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C9" s="1">
-        <v>86</v>
+      <c r="C9" s="5">
+        <v>85.8</v>
       </c>
       <c r="D9" s="2">
+        <v>8.4480329534398005E-2</v>
+      </c>
+      <c r="E9">
         <v>7.1369260782395702E-3</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9">
         <v>0.372</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9">
+        <v>7.1087914481514594E-2</v>
+      </c>
+      <c r="H9">
+        <v>0.45229282525868603</v>
+      </c>
+      <c r="I9">
+        <v>4.9273163083359599E-2</v>
+      </c>
+      <c r="J9">
+        <v>0.461188960298412</v>
+      </c>
+      <c r="K9">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="G9" s="1">
+      <c r="L9" s="6">
         <v>22.6</v>
       </c>
-      <c r="H9" s="3">
+      <c r="M9">
         <v>1.42571515443655E-2</v>
       </c>
-      <c r="I9" s="1">
+      <c r="N9">
         <v>0.20599999999999999</v>
       </c>
-      <c r="J9">
+      <c r="O9">
+        <v>-0.123971870928967</v>
+      </c>
+      <c r="P9">
+        <v>0.188797211385547</v>
+      </c>
+      <c r="Q9">
+        <v>-8.8349300114750604E-2</v>
+      </c>
+      <c r="R9">
+        <v>0.18326440620267301</v>
+      </c>
+      <c r="S9">
+        <v>-0.11940331462888901</v>
+      </c>
+      <c r="T9">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K9">
+      <c r="U9" s="6">
         <v>10.8</v>
       </c>
-      <c r="L9" s="4">
+      <c r="V9">
+        <v>5.89968712834706E-2</v>
+      </c>
+      <c r="W9">
         <v>3.4806308212385101E-3</v>
       </c>
-      <c r="M9">
+      <c r="X9">
         <v>0.53300000000000003</v>
       </c>
-      <c r="N9">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="O9">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="P9" s="4">
-        <v>0.105120554093789</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y9">
+        <v>9.53935444432122E-2</v>
+      </c>
+      <c r="Z9">
+        <v>0.31268498474676298</v>
+      </c>
+      <c r="AA9">
+        <v>5.90107943643704E-2</v>
+      </c>
+      <c r="AB9">
+        <v>0.35333908578726497</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="C10" s="1">
-        <v>86</v>
+      <c r="C10" s="5">
+        <v>85.7</v>
       </c>
       <c r="D10" s="2">
+        <v>-5.7594303563823099E-2</v>
+      </c>
+      <c r="E10">
         <v>3.3171038030043198E-3</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10">
         <v>0.53</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10">
+        <v>-6.3520406940764093E-2</v>
+      </c>
+      <c r="H10">
+        <v>0.48882984362436199</v>
+      </c>
+      <c r="I10">
+        <v>-3.88008283713051E-2</v>
+      </c>
+      <c r="J10">
+        <v>0.55026910464198997</v>
+      </c>
+      <c r="K10">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="L10" s="6">
         <v>21.4</v>
       </c>
-      <c r="H10" s="3">
+      <c r="M10">
         <v>1.66465117480935E-2</v>
       </c>
-      <c r="I10" s="1">
+      <c r="N10">
         <v>0.158</v>
       </c>
-      <c r="J10">
+      <c r="O10">
+        <v>-0.133996962910849</v>
+      </c>
+      <c r="P10">
+        <v>0.142843595129023</v>
+      </c>
+      <c r="Q10">
+        <v>-8.7815272415742898E-2</v>
+      </c>
+      <c r="R10">
+        <v>0.16889205344191299</v>
+      </c>
+      <c r="S10">
+        <v>-0.12902136159603</v>
+      </c>
+      <c r="T10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="K10">
+      <c r="U10" s="6">
         <v>12.6</v>
       </c>
-      <c r="L10" s="4">
+      <c r="V10">
+        <v>0.13821928295265601</v>
+      </c>
+      <c r="W10">
         <v>1.9104570179946601E-2</v>
       </c>
-      <c r="M10">
+      <c r="X10">
         <v>0.13100000000000001</v>
       </c>
-      <c r="N10">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="O10">
-        <v>9.6</v>
-      </c>
-      <c r="P10" s="4">
-        <v>2.45855792720889E-2</v>
-      </c>
-      <c r="Q10">
-        <v>8.5999999999999993E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y10">
+        <v>0.13634562299785899</v>
+      </c>
+      <c r="Z10">
+        <v>0.135907141729639</v>
+      </c>
+      <c r="AA10">
+        <v>8.8346788407048904E-2</v>
+      </c>
+      <c r="AB10">
+        <v>0.15162331266231899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="C11" s="1">
-        <v>86</v>
+      <c r="C11" s="5">
+        <v>86.1</v>
       </c>
       <c r="D11" s="2">
+        <v>-7.9994866456063393E-2</v>
+      </c>
+      <c r="E11">
         <v>6.3991786593226001E-3</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11">
         <v>0.38100000000000001</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11">
+        <v>-8.6716556554243596E-2</v>
+      </c>
+      <c r="H11">
+        <v>0.34224133781959498</v>
+      </c>
+      <c r="I11">
+        <v>-5.6980136707147903E-2</v>
+      </c>
+      <c r="J11">
+        <v>0.38036266202552399</v>
+      </c>
+      <c r="K11">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="G11" s="1">
+      <c r="L11" s="6">
         <v>22</v>
       </c>
-      <c r="H11" s="3">
+      <c r="M11">
         <v>1.32674846709446E-2</v>
       </c>
-      <c r="I11" s="1">
+      <c r="N11">
         <v>0.20599999999999999</v>
       </c>
-      <c r="J11">
+      <c r="O11">
+        <v>-0.12397240251809</v>
+      </c>
+      <c r="P11">
+        <v>0.173678719192564</v>
+      </c>
+      <c r="Q11">
+        <v>-8.8029463991782297E-2</v>
+      </c>
+      <c r="R11">
+        <v>0.168781986839216</v>
+      </c>
+      <c r="S11">
+        <v>-0.115184567850665</v>
+      </c>
+      <c r="T11">
         <v>-2E-3</v>
       </c>
-      <c r="K11">
+      <c r="U11" s="6">
         <v>12.9</v>
       </c>
-      <c r="L11" s="4">
+      <c r="V11">
+        <v>-2.76762490063431E-2</v>
+      </c>
+      <c r="W11">
         <v>7.6597475906103895E-4</v>
       </c>
-      <c r="M11">
+      <c r="X11">
         <v>0.76200000000000001</v>
       </c>
-      <c r="N11">
-        <v>1E-3</v>
-      </c>
-      <c r="O11">
-        <v>9.6</v>
-      </c>
-      <c r="P11" s="4">
-        <v>1.1130516034970599E-3</v>
-      </c>
-      <c r="Q11">
-        <v>0.71499999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y11">
+        <v>-7.3788910184792496E-3</v>
+      </c>
+      <c r="Z11">
+        <v>0.93570870775967196</v>
+      </c>
+      <c r="AA11">
+        <v>-7.7235773066771799E-3</v>
+      </c>
+      <c r="AB11">
+        <v>0.90137574180158198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C12" s="1">
-        <v>87</v>
+      <c r="C12" s="5">
+        <v>86.8</v>
       </c>
       <c r="D12" s="2">
+        <v>0.118848061460215</v>
+      </c>
+      <c r="E12">
         <v>1.4124861712842799E-2</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12">
         <v>0.192</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12">
+        <v>9.9744778335440695E-2</v>
+      </c>
+      <c r="H12">
+        <v>0.27434813733703201</v>
+      </c>
+      <c r="I12">
+        <v>7.3726360117501402E-2</v>
+      </c>
+      <c r="J12">
+        <v>0.25347814051193401</v>
+      </c>
+      <c r="K12">
         <v>-2.1999999999999999E-2</v>
       </c>
-      <c r="G12" s="1">
+      <c r="L12" s="6">
         <v>20</v>
       </c>
-      <c r="H12" s="3">
+      <c r="M12">
         <v>6.4187238060817206E-2</v>
       </c>
-      <c r="I12" s="1">
+      <c r="N12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J12">
+      <c r="O12">
+        <v>-0.26360752559753398</v>
+      </c>
+      <c r="P12">
+        <v>3.3490336758006801E-3</v>
+      </c>
+      <c r="Q12">
+        <v>-0.175979306152968</v>
+      </c>
+      <c r="R12">
+        <v>5.6210279018740197E-3</v>
+      </c>
+      <c r="S12">
+        <v>-0.25335200425656201</v>
+      </c>
+      <c r="T12">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="K12">
+      <c r="U12" s="6">
         <v>14.4</v>
       </c>
-      <c r="L12" s="4">
+      <c r="V12">
+        <v>0.24223088946697199</v>
+      </c>
+      <c r="W12">
         <v>5.8675803811960997E-2</v>
       </c>
-      <c r="M12">
+      <c r="X12">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="P12" s="4">
-        <v>3.4870479790394298E-4</v>
-      </c>
-      <c r="Q12">
-        <v>0.83799999999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y12">
+        <v>0.25570479003312901</v>
+      </c>
+      <c r="Z12">
+        <v>4.4733850229669797E-3</v>
+      </c>
+      <c r="AA12">
+        <v>0.17089037082504799</v>
+      </c>
+      <c r="AB12">
+        <v>5.2985465626629296E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="C13" s="1">
-        <v>86</v>
+      <c r="C13" s="5">
+        <v>86.1</v>
       </c>
       <c r="D13" s="2">
+        <v>-0.16627993718119999</v>
+      </c>
+      <c r="E13">
         <v>2.76490175089904E-2</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13">
+        <v>-0.156277997785916</v>
+      </c>
+      <c r="H13">
+        <v>8.3045920330510503E-2</v>
+      </c>
+      <c r="I13">
+        <v>-0.10223090517740201</v>
+      </c>
+      <c r="J13">
+        <v>0.113413419706565</v>
+      </c>
+      <c r="K13">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="G13" s="1">
+      <c r="L13" s="6">
         <v>20.6</v>
       </c>
-      <c r="H13" s="3">
+      <c r="M13">
         <v>1.8165511536031201E-2</v>
       </c>
-      <c r="I13" s="1">
+      <c r="N13">
         <v>0.13600000000000001</v>
       </c>
-      <c r="J13">
+      <c r="O13">
+        <v>-0.14268225392679401</v>
+      </c>
+      <c r="P13">
+        <v>0.11391220993067599</v>
+      </c>
+      <c r="Q13">
+        <v>-9.5375684606081396E-2</v>
+      </c>
+      <c r="R13">
+        <v>0.132597631561747</v>
+      </c>
+      <c r="S13">
+        <v>-0.13477949226804101</v>
+      </c>
+      <c r="T13">
         <v>2E-3</v>
       </c>
-      <c r="K13">
+      <c r="U13" s="6">
         <v>15.5</v>
       </c>
-      <c r="L13" s="4">
+      <c r="V13">
+        <v>2.68630519342473E-2</v>
+      </c>
+      <c r="W13">
         <v>7.2162355922222898E-4</v>
       </c>
-      <c r="M13">
+      <c r="X13">
         <v>0.76700000000000002</v>
       </c>
-      <c r="N13">
-        <v>-2E-3</v>
-      </c>
-      <c r="O13">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="P13" s="4">
-        <v>4.6519099384493296E-3</v>
-      </c>
-      <c r="Q13">
-        <v>0.45200000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y13">
+        <v>5.0619127577299999E-2</v>
+      </c>
+      <c r="Z13">
+        <v>0.57662577229207301</v>
+      </c>
+      <c r="AA13">
+        <v>2.95217528333034E-2</v>
+      </c>
+      <c r="AB13">
+        <v>0.62852475949535003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1">
         <v>-1E-3</v>
       </c>
-      <c r="C14" s="1">
-        <v>85</v>
+      <c r="C14" s="5">
+        <v>85.1</v>
       </c>
       <c r="D14" s="2">
+        <v>-1.35102163012388E-2</v>
+      </c>
+      <c r="E14">
         <v>1.8252594450618399E-4</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14">
         <v>0.88700000000000001</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14">
+        <v>-1.3427228036528001E-3</v>
+      </c>
+      <c r="H14">
+        <v>0.98868767982968297</v>
+      </c>
+      <c r="I14">
+        <v>5.6774413194809002E-3</v>
+      </c>
+      <c r="J14">
+        <v>0.93465466338083703</v>
+      </c>
+      <c r="K14">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="L14" s="6">
         <v>19</v>
       </c>
-      <c r="H14" s="3">
+      <c r="M14">
         <v>3.11622919391157E-2</v>
       </c>
-      <c r="I14" s="1">
+      <c r="N14">
         <v>0.06</v>
       </c>
-      <c r="J14">
+      <c r="O14">
+        <v>-0.20501537576901799</v>
+      </c>
+      <c r="P14">
+        <v>2.8659436353543101E-2</v>
+      </c>
+      <c r="Q14">
+        <v>-0.13461759896134901</v>
+      </c>
+      <c r="R14">
+        <v>4.1192508658862398E-2</v>
+      </c>
+      <c r="S14">
+        <v>-0.176528445127451</v>
+      </c>
+      <c r="T14">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="K14">
+      <c r="U14" s="6">
         <v>16.8</v>
       </c>
-      <c r="L14" s="4">
+      <c r="V14">
+        <v>9.1384660784935207E-2</v>
+      </c>
+      <c r="W14">
         <v>8.3511562267776195E-3</v>
       </c>
-      <c r="M14">
+      <c r="X14">
         <v>0.33400000000000002</v>
       </c>
-      <c r="N14">
-        <v>-2E-3</v>
-      </c>
-      <c r="O14">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="P14" s="4">
-        <v>7.4721467900025198E-3</v>
-      </c>
-      <c r="Q14">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y14">
+        <v>8.2084701109437594E-2</v>
+      </c>
+      <c r="Z14">
+        <v>0.385267100496262</v>
+      </c>
+      <c r="AA14">
+        <v>5.9321377492603897E-2</v>
+      </c>
+      <c r="AB14">
+        <v>0.35080456886800498</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="C15" s="1">
-        <v>88</v>
+      <c r="C15" s="5">
+        <v>87.7</v>
       </c>
       <c r="D15" s="2">
+        <v>-9.0600177995668399E-2</v>
+      </c>
+      <c r="E15">
         <v>8.2083922528564095E-3</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15">
         <v>0.32300000000000001</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15">
+        <v>-0.100589096213198</v>
+      </c>
+      <c r="H15">
+        <v>0.272299791726275</v>
+      </c>
+      <c r="I15">
+        <v>-7.5540340175179702E-2</v>
+      </c>
+      <c r="J15">
+        <v>0.24745147587564201</v>
+      </c>
+      <c r="K15">
         <v>-2.3E-2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="L15" s="6">
         <v>21.1</v>
       </c>
-      <c r="H15" s="3">
+      <c r="M15">
         <v>8.3070618012968098E-2</v>
       </c>
-      <c r="I15" s="1">
+      <c r="N15">
         <v>1E-3</v>
       </c>
-      <c r="J15">
+      <c r="O15">
+        <v>-0.30409413536601099</v>
+      </c>
+      <c r="P15">
+        <v>6.9640620849662795E-4</v>
+      </c>
+      <c r="Q15">
+        <v>-0.21470608029808</v>
+      </c>
+      <c r="R15">
+        <v>8.1574150776559198E-4</v>
+      </c>
+      <c r="S15">
+        <v>-0.28821973911057303</v>
+      </c>
+      <c r="T15">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="K15">
+      <c r="U15" s="6">
         <v>11</v>
       </c>
-      <c r="L15" s="4">
+      <c r="V15">
+        <v>0.15645761048134901</v>
+      </c>
+      <c r="W15">
         <v>2.44789838775346E-2</v>
       </c>
-      <c r="M15">
+      <c r="X15">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="N15">
-        <v>-1E-3</v>
-      </c>
-      <c r="O15">
-        <v>9.9</v>
-      </c>
-      <c r="P15" s="4">
-        <v>1.52358278229625E-3</v>
-      </c>
-      <c r="Q15">
-        <v>0.67100000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y15">
+        <v>0.17442008161613901</v>
+      </c>
+      <c r="Z15">
+        <v>5.5696921141978398E-2</v>
+      </c>
+      <c r="AA15">
+        <v>0.11163176999421701</v>
+      </c>
+      <c r="AB15">
+        <v>6.9919012403598199E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="C16" s="1">
-        <v>87</v>
+      <c r="C16" s="5">
+        <v>86.8</v>
       </c>
       <c r="D16" s="2">
+        <v>-3.8446041501452803E-2</v>
+      </c>
+      <c r="E16">
         <v>1.4780981071317301E-3</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16">
         <v>0.69299999999999995</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16">
+        <v>-5.6567910526867597E-2</v>
+      </c>
+      <c r="H16">
+        <v>0.56090599604805702</v>
+      </c>
+      <c r="I16">
+        <v>-4.0857198406294003E-2</v>
+      </c>
+      <c r="J16">
+        <v>0.55595420745660096</v>
+      </c>
+      <c r="K16">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="G16" s="1">
+      <c r="L16" s="6">
         <v>19.600000000000001</v>
       </c>
-      <c r="H16" s="3">
+      <c r="M16">
         <v>3.5280056769531401E-2</v>
       </c>
-      <c r="I16" s="1">
+      <c r="N16">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="J16">
+      <c r="O16">
+        <v>-0.212458677836629</v>
+      </c>
+      <c r="P16">
+        <v>2.7278432355986301E-2</v>
+      </c>
+      <c r="Q16">
+        <v>-0.144165610324271</v>
+      </c>
+      <c r="R16">
+        <v>3.3865215952970998E-2</v>
+      </c>
+      <c r="S16">
+        <v>-0.18782986122959999</v>
+      </c>
+      <c r="T16">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="K16">
+      <c r="U16" s="6">
         <v>13.5</v>
       </c>
-      <c r="L16" s="4">
+      <c r="V16">
+        <v>0.100070448011942</v>
+      </c>
+      <c r="W16">
         <v>1.00140945653112E-2</v>
       </c>
-      <c r="M16">
+      <c r="X16">
         <v>0.30299999999999999</v>
       </c>
-      <c r="N16">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="O16">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="P16" s="4">
-        <v>1.2523740514460899E-2</v>
-      </c>
-      <c r="Q16">
-        <v>0.249</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y16">
+        <v>0.11426638817767699</v>
+      </c>
+      <c r="Z16">
+        <v>0.23898217783602699</v>
+      </c>
+      <c r="AA16">
+        <v>7.6370262534554395E-2</v>
+      </c>
+      <c r="AB16">
+        <v>0.24274504347773801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="C17" s="1">
-        <v>88</v>
+      <c r="C17" s="5">
+        <v>88.4</v>
       </c>
       <c r="D17" s="2">
+        <v>-9.7304179071479299E-2</v>
+      </c>
+      <c r="E17">
         <v>9.4681032647832009E-3</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17">
         <v>0.28399999999999997</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17">
+        <v>-0.12673456583196599</v>
+      </c>
+      <c r="H17">
+        <v>0.16246103032515599</v>
+      </c>
+      <c r="I17">
+        <v>-9.2871980264391002E-2</v>
+      </c>
+      <c r="J17">
+        <v>0.143350881435686</v>
+      </c>
+      <c r="K17">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="G17" s="1">
+      <c r="L17" s="6">
         <v>17.8</v>
       </c>
-      <c r="H17" s="3">
+      <c r="M17">
         <v>7.6496991717342797E-2</v>
       </c>
-      <c r="I17" s="1">
+      <c r="N17">
         <v>2E-3</v>
       </c>
-      <c r="J17">
+      <c r="O17">
+        <v>-0.28872787876003803</v>
+      </c>
+      <c r="P17">
+        <v>1.2006912995540799E-3</v>
+      </c>
+      <c r="Q17">
+        <v>-0.18870884995103701</v>
+      </c>
+      <c r="R17">
+        <v>2.7584708471461599E-3</v>
+      </c>
+      <c r="S17">
+        <v>-0.276580895430872</v>
+      </c>
+      <c r="T17">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="K17">
+      <c r="U17" s="6">
         <v>13.8</v>
       </c>
-      <c r="L17" s="4">
+      <c r="V17">
+        <v>0.103556182250294</v>
+      </c>
+      <c r="W17">
         <v>1.07238828822566E-2</v>
       </c>
-      <c r="M17">
+      <c r="X17">
         <v>0.254</v>
       </c>
-      <c r="N17">
-        <v>1E-3</v>
-      </c>
-      <c r="O17">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="P17" s="4">
-        <v>6.0158912851226997E-4</v>
-      </c>
-      <c r="Q17">
-        <v>0.78800000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y17">
+        <v>9.1541983755841203E-2</v>
+      </c>
+      <c r="Z17">
+        <v>0.31393487858060698</v>
+      </c>
+      <c r="AA17">
+        <v>5.8541147146582401E-2</v>
+      </c>
+      <c r="AB17">
+        <v>0.33830321111079298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>-2E-3</v>
       </c>
-      <c r="C18" s="1">
-        <v>87</v>
+      <c r="C18" s="5">
+        <v>86.6</v>
       </c>
       <c r="D18" s="2">
+        <v>-3.5798845772769899E-2</v>
+      </c>
+      <c r="E18">
         <v>1.2815573586627499E-3</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18">
         <v>0.69299999999999995</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18">
+        <v>-3.01840733575073E-2</v>
+      </c>
+      <c r="H18">
+        <v>0.73929478439893903</v>
+      </c>
+      <c r="I18">
+        <v>-1.82399017385028E-2</v>
+      </c>
+      <c r="J18">
+        <v>0.77918089801864199</v>
+      </c>
+      <c r="K18">
         <v>-8.0000000000000002E-3</v>
       </c>
-      <c r="G18" s="1">
+      <c r="L18" s="6">
         <v>19.3</v>
       </c>
-      <c r="H18" s="3">
+      <c r="M18">
         <v>1.06325623698122E-2</v>
       </c>
-      <c r="I18" s="1">
+      <c r="N18">
         <v>0.254</v>
       </c>
-      <c r="J18">
+      <c r="O18">
+        <v>-0.102543208764983</v>
+      </c>
+      <c r="P18">
+        <v>0.25708886531819097</v>
+      </c>
+      <c r="Q18">
+        <v>-6.4612544741141906E-2</v>
+      </c>
+      <c r="R18">
+        <v>0.308857165546438</v>
+      </c>
+      <c r="S18">
+        <v>-0.10311431699726401</v>
+      </c>
+      <c r="T18">
         <v>1E-3</v>
       </c>
-      <c r="K18">
+      <c r="U18" s="6">
         <v>15.2</v>
       </c>
-      <c r="L18" s="4">
+      <c r="V18">
+        <v>1.32802183646365E-2</v>
+      </c>
+      <c r="W18">
         <v>1.76364199812484E-4</v>
       </c>
-      <c r="M18">
+      <c r="X18">
         <v>0.88400000000000001</v>
       </c>
-      <c r="N18">
-        <v>-1E-3</v>
-      </c>
-      <c r="O18">
-        <v>9.6</v>
-      </c>
-      <c r="P18" s="4">
-        <v>6.2417351698673695E-4</v>
-      </c>
-      <c r="Q18">
-        <v>0.78300000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y18">
+        <v>2.48371751962152E-2</v>
+      </c>
+      <c r="Z18">
+        <v>0.78422583472176399</v>
+      </c>
+      <c r="AA18">
+        <v>1.6916923516793501E-2</v>
+      </c>
+      <c r="AB18">
+        <v>0.78219904474672197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="C19" s="1">
-        <v>87</v>
+      <c r="C19" s="5">
+        <v>86.7</v>
       </c>
       <c r="D19" s="2">
+        <v>-0.30234870810543502</v>
+      </c>
+      <c r="E19">
         <v>9.1414741293109697E-2</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19">
         <v>1E-3</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19">
+        <v>-0.32186426161210402</v>
+      </c>
+      <c r="H19">
+        <v>3.18160042595043E-4</v>
+      </c>
+      <c r="I19">
+        <v>-0.22475019739729801</v>
+      </c>
+      <c r="J19">
+        <v>5.9486905126149802E-4</v>
+      </c>
+      <c r="K19">
         <v>2E-3</v>
       </c>
-      <c r="G19" s="1">
+      <c r="L19" s="6">
         <v>16.600000000000001</v>
       </c>
-      <c r="H19" s="3">
+      <c r="M19">
         <v>4.0799264275559498E-4</v>
       </c>
-      <c r="I19" s="1">
+      <c r="N19">
         <v>0.82599999999999996</v>
       </c>
-      <c r="J19">
+      <c r="O19">
+        <v>2.9720217129209701E-3</v>
+      </c>
+      <c r="P19">
+        <v>0.97419057383173202</v>
+      </c>
+      <c r="Q19">
+        <v>7.4121596612199501E-3</v>
+      </c>
+      <c r="R19">
+        <v>0.91010512250042797</v>
+      </c>
+      <c r="S19">
+        <v>2.0198827756966999E-2</v>
+      </c>
+      <c r="T19">
         <v>1.2E-2</v>
       </c>
-      <c r="K19">
+      <c r="U19" s="6">
         <v>17.3</v>
       </c>
-      <c r="L19" s="4">
+      <c r="V19">
+        <v>0.196429067060616</v>
+      </c>
+      <c r="W19">
         <v>3.8584378386305102E-2</v>
       </c>
-      <c r="M19">
+      <c r="X19">
         <v>3.1E-2</v>
       </c>
-      <c r="N19">
-        <v>1E-3</v>
-      </c>
-      <c r="O19">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="P19" s="4">
-        <v>1.3115374944512299E-3</v>
-      </c>
-      <c r="Q19">
-        <v>0.69299999999999995</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y19">
+        <v>0.203836585260389</v>
+      </c>
+      <c r="Z19">
+        <v>2.4927309015832701E-2</v>
+      </c>
+      <c r="AA19">
+        <v>0.13656723148520999</v>
+      </c>
+      <c r="AB19">
+        <v>2.6559795057542999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="1">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C20" s="1">
-        <v>87</v>
+      <c r="C20" s="5">
+        <v>86.5</v>
       </c>
       <c r="D20" s="2">
+        <v>-0.17063003930901099</v>
+      </c>
+      <c r="E20">
         <v>2.9114610314615999E-2</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20">
+        <v>-0.17313910072663</v>
+      </c>
+      <c r="H20">
+        <v>5.96954964212279E-2</v>
+      </c>
+      <c r="I20">
+        <v>-0.120557398113232</v>
+      </c>
+      <c r="J20">
+        <v>6.6617050247880394E-2</v>
+      </c>
+      <c r="K20">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="G20" s="1">
+      <c r="L20" s="6">
         <v>17.600000000000001</v>
       </c>
-      <c r="H20" s="3">
+      <c r="M20">
         <v>5.15716482282469E-3</v>
       </c>
-      <c r="I20" s="1">
+      <c r="N20">
         <v>0.438</v>
       </c>
-      <c r="J20">
+      <c r="O20">
+        <v>-5.77452114907058E-2</v>
+      </c>
+      <c r="P20">
+        <v>0.53276047596421705</v>
+      </c>
+      <c r="Q20">
+        <v>-3.7529297272345802E-2</v>
+      </c>
+      <c r="R20">
+        <v>0.56296514615476201</v>
+      </c>
+      <c r="S20">
+        <v>-7.1813402807723803E-2</v>
+      </c>
+      <c r="T20">
         <v>0.01</v>
       </c>
-      <c r="K20">
+      <c r="U20" s="6">
         <v>17.600000000000001</v>
       </c>
-      <c r="L20" s="4">
+      <c r="V20">
+        <v>0.13829840629016901</v>
+      </c>
+      <c r="W20">
         <v>1.9126449182401101E-2</v>
       </c>
-      <c r="M20">
+      <c r="X20">
         <v>0.13400000000000001</v>
       </c>
-      <c r="N20">
-        <v>-1E-3</v>
-      </c>
-      <c r="O20">
-        <v>9.1</v>
-      </c>
-      <c r="P20" s="4">
-        <v>1.12710766663748E-3</v>
-      </c>
-      <c r="Q20">
-        <v>0.71699999999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y20">
+        <v>0.12846173156641499</v>
+      </c>
+      <c r="Z20">
+        <v>0.16382053463297</v>
+      </c>
+      <c r="AA20">
+        <v>8.6046016637995298E-2</v>
+      </c>
+      <c r="AB20">
+        <v>0.16606260248518201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C21" s="1">
-        <v>88</v>
+      <c r="C21" s="5">
+        <v>87.6</v>
       </c>
       <c r="D21" s="2">
+        <v>0.15467473707680801</v>
+      </c>
+      <c r="E21">
         <v>2.39242742897917E-2</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21">
         <v>0.1</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21">
+        <v>0.14041512552206001</v>
+      </c>
+      <c r="H21">
+        <v>0.13619957755290499</v>
+      </c>
+      <c r="I21">
+        <v>9.8889799529320394E-2</v>
+      </c>
+      <c r="J21">
+        <v>0.142406480520017</v>
+      </c>
+      <c r="K21">
         <v>-3.5999999999999997E-2</v>
       </c>
-      <c r="G21" s="1">
+      <c r="L21" s="6">
         <v>19</v>
       </c>
-      <c r="H21" s="3">
+      <c r="M21">
         <v>0.18246728424533701</v>
       </c>
-      <c r="I21" s="1">
+      <c r="N21">
         <v>0</v>
       </c>
-      <c r="J21">
+      <c r="O21">
+        <v>-0.420992604466362</v>
+      </c>
+      <c r="P21" s="4">
+        <v>3.09989418041187E-6</v>
+      </c>
+      <c r="Q21">
+        <v>-0.29564710279207101</v>
+      </c>
+      <c r="R21" s="4">
+        <v>7.2104148167277504E-6</v>
+      </c>
+      <c r="S21">
+        <v>-0.42716189465510501</v>
+      </c>
+      <c r="T21">
         <v>1E-3</v>
       </c>
-      <c r="K21">
+      <c r="U21" s="6">
         <v>11.3</v>
       </c>
-      <c r="L21" s="4">
+      <c r="V21">
+        <v>2.3825076784374701E-2</v>
+      </c>
+      <c r="W21">
         <v>5.6763428378126001E-4</v>
       </c>
-      <c r="M21">
+      <c r="X21">
         <v>0.80100000000000005</v>
       </c>
-      <c r="N21">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="O21">
-        <v>10</v>
-      </c>
-      <c r="P21" s="4">
-        <v>1.0085898442722599E-2</v>
-      </c>
-      <c r="Q21">
-        <v>0.28799999999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y21">
+        <v>1.1356893626213701E-2</v>
+      </c>
+      <c r="Z21">
+        <v>0.90454180280011398</v>
+      </c>
+      <c r="AA21">
+        <v>4.9724204314205702E-3</v>
+      </c>
+      <c r="AB21">
+        <v>0.93948438612039997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="1">
         <v>-2E-3</v>
       </c>
-      <c r="C22" s="1">
-        <v>89</v>
+      <c r="C22" s="5">
+        <v>88.7</v>
       </c>
       <c r="D22" s="2">
+        <v>-2.9300096499706201E-2</v>
+      </c>
+      <c r="E22">
         <v>8.5849565489226599E-4</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22">
         <v>0.75700000000000001</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22">
+        <v>-5.9401556087820502E-2</v>
+      </c>
+      <c r="H22">
+        <v>0.53013488502518402</v>
+      </c>
+      <c r="I22">
+        <v>-3.9464865285687399E-2</v>
+      </c>
+      <c r="J22">
+        <v>0.55985603825326702</v>
+      </c>
+      <c r="K22">
         <v>1.2E-2</v>
       </c>
-      <c r="G22" s="1">
+      <c r="L22" s="6">
         <v>19.600000000000001</v>
       </c>
-      <c r="H22" s="3">
+      <c r="M22">
         <v>2.6830091185623E-2</v>
       </c>
-      <c r="I22" s="1">
+      <c r="N22">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="J22">
+      <c r="O22">
+        <v>0.113366401378037</v>
+      </c>
+      <c r="P22">
+        <v>0.22976736501887801</v>
+      </c>
+      <c r="Q22">
+        <v>8.8631978909545106E-2</v>
+      </c>
+      <c r="R22">
+        <v>0.18550465005516201</v>
+      </c>
+      <c r="S22">
+        <v>0.16379893523958899</v>
+      </c>
+      <c r="T22">
         <v>-2E-3</v>
       </c>
-      <c r="K22">
+      <c r="U22" s="6">
         <v>13.1</v>
       </c>
-      <c r="L22" s="4">
+      <c r="V22">
+        <v>-3.22183323206588E-2</v>
+      </c>
+      <c r="W22">
         <v>1.0380209375244801E-3</v>
       </c>
-      <c r="M22">
+      <c r="X22">
         <v>0.73399999999999999</v>
       </c>
-      <c r="N22">
-        <v>2E-3</v>
-      </c>
-      <c r="O22">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="P22" s="4">
-        <v>3.7264330922285299E-3</v>
-      </c>
-      <c r="Q22">
-        <v>0.51900000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y22">
+        <v>-4.0482058499429603E-2</v>
+      </c>
+      <c r="Z22">
+        <v>0.66891175568442096</v>
+      </c>
+      <c r="AA22">
+        <v>-2.81230662866114E-2</v>
+      </c>
+      <c r="AB22">
+        <v>0.65934937578485597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="1">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="C23" s="1">
-        <v>87</v>
+      <c r="C23" s="5">
+        <v>86.9</v>
       </c>
       <c r="D23" s="2">
+        <v>-5.7360906710347402E-2</v>
+      </c>
+      <c r="E23">
         <v>3.29027361863388E-3</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23">
         <v>0.54400000000000004</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23">
+        <v>-3.3822467745045E-2</v>
+      </c>
+      <c r="H23">
+        <v>0.72090648849153605</v>
+      </c>
+      <c r="I23">
+        <v>-1.8533175727546099E-2</v>
+      </c>
+      <c r="J23">
+        <v>0.78331992496152103</v>
+      </c>
+      <c r="K23">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G23" s="1">
+      <c r="L23" s="6">
         <v>17.3</v>
       </c>
-      <c r="H23" s="3">
+      <c r="M23">
         <v>7.7866887980828602E-3</v>
       </c>
-      <c r="I23" s="1">
+      <c r="N23">
         <v>0.35099999999999998</v>
       </c>
-      <c r="J23">
+      <c r="O23">
+        <v>7.2527687922120804E-2</v>
+      </c>
+      <c r="P23">
+        <v>0.44316457506247398</v>
+      </c>
+      <c r="Q23">
+        <v>5.6805214944822303E-2</v>
+      </c>
+      <c r="R23">
+        <v>0.39379554755942098</v>
+      </c>
+      <c r="S23">
+        <v>8.8242216643071095E-2</v>
+      </c>
+      <c r="T23">
         <v>1.6E-2</v>
       </c>
-      <c r="K23">
+      <c r="U23" s="6">
         <v>16.399999999999999</v>
       </c>
-      <c r="L23" s="4">
+      <c r="V23">
+        <v>0.211465984812228</v>
+      </c>
+      <c r="W23">
         <v>4.4717862732604301E-2</v>
       </c>
-      <c r="M23">
+      <c r="X23">
         <v>2.4E-2</v>
       </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="P23" s="4">
-        <v>8.7195095206382703E-5</v>
-      </c>
-      <c r="Q23">
-        <v>0.92100000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y23">
+        <v>0.19169393772635601</v>
+      </c>
+      <c r="Z23">
+        <v>4.1036214451997302E-2</v>
+      </c>
+      <c r="AA23">
+        <v>0.126242237546804</v>
+      </c>
+      <c r="AB23">
+        <v>4.6756579361133199E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="1">
         <v>-0.01</v>
       </c>
-      <c r="C24" s="1">
-        <v>87</v>
+      <c r="C24" s="5">
+        <v>87.2</v>
       </c>
       <c r="D24" s="2">
+        <v>-0.15941749719699499</v>
+      </c>
+      <c r="E24">
         <v>2.5413938412560198E-2</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24">
+        <v>-0.199509196212553</v>
+      </c>
+      <c r="H24">
+        <v>2.6315490175235701E-2</v>
+      </c>
+      <c r="I24">
+        <v>-0.144626594467261</v>
+      </c>
+      <c r="J24">
+        <v>2.52398546421203E-2</v>
+      </c>
+      <c r="K24">
         <v>1E-3</v>
       </c>
-      <c r="G24" s="1">
+      <c r="L24" s="6">
         <v>17.600000000000001</v>
       </c>
-      <c r="H24" s="3">
+      <c r="M24">
         <v>2.7571152798489001E-4</v>
       </c>
-      <c r="I24" s="1">
+      <c r="N24">
         <v>0.85499999999999998</v>
       </c>
-      <c r="J24">
+      <c r="O24">
+        <v>-1.9956182833878101E-2</v>
+      </c>
+      <c r="P24">
+        <v>0.82587587027062204</v>
+      </c>
+      <c r="Q24">
+        <v>-4.57218081219122E-3</v>
+      </c>
+      <c r="R24">
+        <v>0.94444926654208206</v>
+      </c>
+      <c r="S24">
+        <v>1.6604563468661598E-2</v>
+      </c>
+      <c r="T24">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="K24">
+      <c r="U24" s="6">
         <v>17.2</v>
       </c>
-      <c r="L24" s="4">
+      <c r="V24">
+        <v>8.4512663597443402E-2</v>
+      </c>
+      <c r="W24">
         <v>7.1423903083348596E-3</v>
       </c>
-      <c r="M24">
+      <c r="X24">
         <v>0.35099999999999998</v>
       </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>9.4</v>
-      </c>
-      <c r="P24" s="4">
-        <v>2.047957714435E-4</v>
-      </c>
-      <c r="Q24">
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y24">
+        <v>4.8893938297451603E-2</v>
+      </c>
+      <c r="Z24">
+        <v>0.589701652166568</v>
+      </c>
+      <c r="AA24">
+        <v>3.9606557717659203E-2</v>
+      </c>
+      <c r="AB24">
+        <v>0.51562671160558704</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="1">
         <v>-1.2E-2</v>
       </c>
-      <c r="C25" s="1">
-        <v>86</v>
+      <c r="C25" s="5">
+        <v>85.6</v>
       </c>
       <c r="D25" s="2">
+        <v>-0.198535272490488</v>
+      </c>
+      <c r="E25">
         <v>3.9416254422878098E-2</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25">
         <v>2.7E-2</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25">
+        <v>-0.19967328333690801</v>
+      </c>
+      <c r="H25">
+        <v>2.6189594182117901E-2</v>
+      </c>
+      <c r="I25">
+        <v>-0.140281214960677</v>
+      </c>
+      <c r="J25">
+        <v>3.0602754582811899E-2</v>
+      </c>
+      <c r="K25">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="G25" s="1">
+      <c r="L25" s="6">
         <v>16.399999999999999</v>
       </c>
-      <c r="H25" s="3">
+      <c r="M25">
         <v>2.8831238536278802E-3</v>
       </c>
-      <c r="I25" s="1">
+      <c r="N25">
         <v>0.55400000000000005</v>
       </c>
-      <c r="J25">
+      <c r="O25">
+        <v>-0.12447981184927601</v>
+      </c>
+      <c r="P25">
+        <v>0.16836575766904199</v>
+      </c>
+      <c r="Q25">
+        <v>-8.1074162241002307E-2</v>
+      </c>
+      <c r="R25">
+        <v>0.20090149049540201</v>
+      </c>
+      <c r="S25">
+        <v>-5.3694728359753897E-2</v>
+      </c>
+      <c r="T25">
         <v>-2E-3</v>
       </c>
-      <c r="K25">
+      <c r="U25" s="6">
         <v>17.8</v>
       </c>
-      <c r="L25" s="4">
+      <c r="V25">
+        <v>-3.4037208371678403E-2</v>
+      </c>
+      <c r="W25">
         <v>1.15853155373702E-3</v>
       </c>
-      <c r="M25">
+      <c r="X25">
         <v>0.70699999999999996</v>
       </c>
-      <c r="N25">
-        <v>2E-3</v>
-      </c>
-      <c r="O25">
-        <v>9</v>
-      </c>
-      <c r="P25" s="4">
-        <v>5.4127081400029402E-3</v>
-      </c>
-      <c r="Q25">
-        <v>0.41699999999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Y25">
+        <v>-1.20409884564995E-2</v>
+      </c>
+      <c r="Z25">
+        <v>0.89440721191898997</v>
+      </c>
+      <c r="AA25">
+        <v>-3.9349424229081099E-3</v>
+      </c>
+      <c r="AB25">
+        <v>0.95005743820150601</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B26">
         <f t="shared" ref="B26:N26" si="0">AVERAGE(B3:B25)</f>
         <v>-4.4347826086956511E-3</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>86.434782608695656</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>2.1400031817898329E-2</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0.32982608695652171</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>-9.5217391304347806E-3</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>20.065217391304355</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>2.9932700917776386E-2</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>0.26573913043478259</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>4.6956521739130435E-3</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="0"/>
-        <v>14.243478260869566</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="0"/>
-        <v>1.3986133878871407E-2</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="0"/>
-        <v>0.40052173913043476</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="0"/>
-        <v>1.2173913043478262E-3</v>
-      </c>
-      <c r="O26">
-        <f>AVERAGE(O3:O25)</f>
-        <v>9.5695652173913057</v>
-      </c>
-      <c r="P26">
-        <f t="shared" ref="P26:Q26" si="1">AVERAGE(P3:P25)</f>
-        <v>9.2968816474342658E-3</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="1"/>
-        <v>0.57578260869565212</v>
-      </c>
+        <v>86.339130434782604</v>
+      </c>
+      <c r="L26" s="6">
+        <v>0</v>
+      </c>
+      <c r="U26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
+  <mergeCells count="3">
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="T1:AB1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:D25 H3:H25 L3:L25 P3:P25">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
+  <conditionalFormatting sqref="D3:D25">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>"0..5"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E26 I3:I26 M3:M26 Q3:Q26">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
-      <formula>0.05</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="between">
-      <formula>0.05</formula>
-      <formula>0.06</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="between">
-      <formula>0.04</formula>
-      <formula>0.04</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3731,11 +4338,11 @@
       <selection activeCell="I130" sqref="I130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3807,7 +4414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1890</v>
       </c>
@@ -3881,7 +4488,7 @@
         <v>85.28</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1891</v>
       </c>
@@ -3955,7 +4562,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1892</v>
       </c>
@@ -4029,7 +4636,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1893</v>
       </c>
@@ -4103,7 +4710,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1894</v>
       </c>
@@ -4177,7 +4784,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1895</v>
       </c>
@@ -4251,7 +4858,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1896</v>
       </c>
@@ -4325,7 +4932,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1897</v>
       </c>
@@ -4399,7 +5006,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1898</v>
       </c>
@@ -4473,7 +5080,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1899</v>
       </c>
@@ -4547,7 +5154,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1900</v>
       </c>
@@ -4621,7 +5228,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1901</v>
       </c>
@@ -4695,7 +5302,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1902</v>
       </c>
@@ -4769,7 +5376,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1903</v>
       </c>
@@ -4843,7 +5450,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1904</v>
       </c>
@@ -4917,7 +5524,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1905</v>
       </c>
@@ -4991,7 +5598,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1906</v>
       </c>
@@ -5065,7 +5672,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1907</v>
       </c>
@@ -5139,7 +5746,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1908</v>
       </c>
@@ -5213,7 +5820,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1909</v>
       </c>
@@ -5287,7 +5894,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1910</v>
       </c>
@@ -5361,7 +5968,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1911</v>
       </c>
@@ -5435,7 +6042,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1912</v>
       </c>
@@ -5509,7 +6116,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1913</v>
       </c>
@@ -5583,7 +6190,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1914</v>
       </c>
@@ -5657,7 +6264,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1915</v>
       </c>
@@ -5731,7 +6338,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1916</v>
       </c>
@@ -5805,7 +6412,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1917</v>
       </c>
@@ -5879,7 +6486,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1918</v>
       </c>
@@ -5953,7 +6560,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1919</v>
       </c>
@@ -6027,7 +6634,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1920</v>
       </c>
@@ -6101,7 +6708,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1921</v>
       </c>
@@ -6175,7 +6782,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1922</v>
       </c>
@@ -6249,7 +6856,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1923</v>
       </c>
@@ -6323,7 +6930,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1924</v>
       </c>
@@ -6397,7 +7004,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1925</v>
       </c>
@@ -6471,7 +7078,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1926</v>
       </c>
@@ -6545,7 +7152,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1927</v>
       </c>
@@ -6619,7 +7226,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1928</v>
       </c>
@@ -6693,7 +7300,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1929</v>
       </c>
@@ -6767,7 +7374,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1930</v>
       </c>
@@ -6841,7 +7448,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1931</v>
       </c>
@@ -6915,7 +7522,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1932</v>
       </c>
@@ -6989,7 +7596,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1933</v>
       </c>
@@ -7063,7 +7670,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1934</v>
       </c>
@@ -7137,7 +7744,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1935</v>
       </c>
@@ -7211,7 +7818,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1936</v>
       </c>
@@ -7285,7 +7892,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1937</v>
       </c>
@@ -7359,7 +7966,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1938</v>
       </c>
@@ -7433,7 +8040,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1939</v>
       </c>
@@ -7507,7 +8114,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1940</v>
       </c>
@@ -7581,7 +8188,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1941</v>
       </c>
@@ -7655,7 +8262,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1942</v>
       </c>
@@ -7729,7 +8336,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1943</v>
       </c>
@@ -7803,7 +8410,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1944</v>
       </c>
@@ -7877,7 +8484,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1945</v>
       </c>
@@ -7951,7 +8558,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1946</v>
       </c>
@@ -8025,7 +8632,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1947</v>
       </c>
@@ -8099,7 +8706,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1948</v>
       </c>
@@ -8173,7 +8780,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1949</v>
       </c>
@@ -8247,7 +8854,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1950</v>
       </c>
@@ -8321,7 +8928,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1951</v>
       </c>
@@ -8395,7 +9002,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>1952</v>
       </c>
@@ -8469,7 +9076,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1953</v>
       </c>
@@ -8543,7 +9150,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1954</v>
       </c>
@@ -8617,7 +9224,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1955</v>
       </c>
@@ -8691,7 +9298,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1956</v>
       </c>
@@ -8765,7 +9372,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>1957</v>
       </c>
@@ -8839,7 +9446,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1958</v>
       </c>
@@ -8913,7 +9520,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1959</v>
       </c>
@@ -8987,7 +9594,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>1960</v>
       </c>
@@ -9061,7 +9668,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1961</v>
       </c>
@@ -9135,7 +9742,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1962</v>
       </c>
@@ -9209,7 +9816,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1963</v>
       </c>
@@ -9283,7 +9890,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1964</v>
       </c>
@@ -9357,7 +9964,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>1965</v>
       </c>
@@ -9431,7 +10038,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1966</v>
       </c>
@@ -9505,7 +10112,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1967</v>
       </c>
@@ -9579,7 +10186,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1968</v>
       </c>
@@ -9653,7 +10260,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1969</v>
       </c>
@@ -9727,7 +10334,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1970</v>
       </c>
@@ -9801,7 +10408,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>1971</v>
       </c>
@@ -9875,7 +10482,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1972</v>
       </c>
@@ -9949,7 +10556,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1973</v>
       </c>
@@ -10023,7 +10630,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>1974</v>
       </c>
@@ -10097,7 +10704,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>1975</v>
       </c>
@@ -10171,7 +10778,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1976</v>
       </c>
@@ -10245,7 +10852,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>1977</v>
       </c>
@@ -10319,7 +10926,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1978</v>
       </c>
@@ -10393,7 +11000,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>1979</v>
       </c>
@@ -10467,7 +11074,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>1980</v>
       </c>
@@ -10541,7 +11148,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>1981</v>
       </c>
@@ -10615,7 +11222,7 @@
         <v>84.91</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>1982</v>
       </c>
@@ -10689,7 +11296,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>1983</v>
       </c>
@@ -10763,7 +11370,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1984</v>
       </c>
@@ -10837,7 +11444,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1985</v>
       </c>
@@ -10911,7 +11518,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>1986</v>
       </c>
@@ -10985,7 +11592,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1987</v>
       </c>
@@ -11059,7 +11666,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>1988</v>
       </c>
@@ -11133,7 +11740,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1989</v>
       </c>
@@ -11207,7 +11814,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>1990</v>
       </c>
@@ -11281,7 +11888,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1991</v>
       </c>
@@ -11355,7 +11962,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1992</v>
       </c>
@@ -11429,7 +12036,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1993</v>
       </c>
@@ -11503,7 +12110,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1994</v>
       </c>
@@ -11577,7 +12184,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1995</v>
       </c>
@@ -11651,7 +12258,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1996</v>
       </c>
@@ -11725,7 +12332,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1997</v>
       </c>
@@ -11799,7 +12406,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1998</v>
       </c>
@@ -11873,7 +12480,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>1999</v>
       </c>
@@ -11947,7 +12554,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2000</v>
       </c>
@@ -12021,7 +12628,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2001</v>
       </c>
@@ -12095,7 +12702,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2002</v>
       </c>
@@ -12169,7 +12776,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2003</v>
       </c>
@@ -12243,7 +12850,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2004</v>
       </c>
@@ -12317,7 +12924,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2005</v>
       </c>
@@ -12391,7 +12998,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2006</v>
       </c>
@@ -12465,7 +13072,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2007</v>
       </c>
@@ -12539,7 +13146,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2008</v>
       </c>
@@ -12613,7 +13220,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2009</v>
       </c>
@@ -12687,7 +13294,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2010</v>
       </c>
@@ -12761,7 +13368,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2011</v>
       </c>
@@ -12835,7 +13442,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2012</v>
       </c>
@@ -12909,7 +13516,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2013</v>
       </c>

</xml_diff>